<commit_message>
full html content added and completed
</commit_message>
<xml_diff>
--- a/site/Book1.xlsx
+++ b/site/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>course overview</t>
   </si>
@@ -114,6 +114,48 @@
   </si>
   <si>
     <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/_Icm84NSZmQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/NyhK2iW0Zm4" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Forms overview</t>
+  </si>
+  <si>
+    <t>Forms (Input Types)</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/m8TeF-Ux-Tg" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/NUVGwUkxwU4" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Form Tag</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/lnCRVkPX7js" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Forms Textarea and Select</t>
+  </si>
+  <si>
+    <t>Body Attributes</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/llH36fGCEUk" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Doctype and Head</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/CrxbN7cv10Y" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/u43z0OKDtSc" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>Next steps</t>
   </si>
 </sst>
 </file>
@@ -483,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +657,62 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>